<commit_message>
merapihkan form tambah dan edit
</commit_message>
<xml_diff>
--- a/media/laporan/2025/06/laporan-pengiriman-barang-20250601-20250630.xlsx
+++ b/media/laporan/2025/06/laporan-pengiriman-barang-20250601-20250630.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
   <si>
     <t>LAPORAN SERVICE AC</t>
   </si>
@@ -26,40 +26,128 @@
     <t>No.</t>
   </si>
   <si>
-    <t>Tanggal</t>
-  </si>
-  <si>
     <t>Nama</t>
   </si>
   <si>
+    <t>PK</t>
+  </si>
+  <si>
+    <t>Teknisi 1</t>
+  </si>
+  <si>
+    <t>Teknisi 2</t>
+  </si>
+  <si>
+    <t>Teknisi 3</t>
+  </si>
+  <si>
+    <t>No Hp</t>
+  </si>
+  <si>
+    <t>Tanggal Perbaikan</t>
+  </si>
+  <si>
+    <t>Deskripsi Kerusakan</t>
+  </si>
+  <si>
+    <t>Merk AC</t>
+  </si>
+  <si>
+    <t>Remot Jenis</t>
+  </si>
+  <si>
     <t>Remot Kode</t>
   </si>
   <si>
-    <t>No Hp</t>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Dadan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abdul Hamid </t>
+  </si>
+  <si>
+    <t>Erik Hasibuan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wage Rudolf Supratman </t>
+  </si>
+  <si>
+    <t>087678987677</t>
   </si>
   <si>
     <t>2025-06-25</t>
   </si>
   <si>
-    <t>Dadan</t>
+    <t>Service AC Rutin</t>
+  </si>
+  <si>
+    <t>Daikin FTC15NV14</t>
+  </si>
+  <si>
+    <t>Original</t>
+  </si>
+  <si>
+    <t>Muhammad Yamin</t>
+  </si>
+  <si>
+    <t>Robert Ed Stewart</t>
+  </si>
+  <si>
+    <t>089976356474</t>
   </si>
   <si>
     <t>2025-06-22</t>
   </si>
   <si>
-    <t>Muhammad Yamin</t>
+    <t xml:space="preserve">Lorem Ipsum is simply dummy text of the printing and typesetting industry.
+</t>
+  </si>
+  <si>
+    <t>Changhong CSC-05NVB</t>
+  </si>
+  <si>
+    <t>Tidak Original</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jihan Fahriza Amalina </t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Abdul Yamin</t>
+  </si>
+  <si>
+    <t>087898876567</t>
   </si>
   <si>
     <t>2025-06-18</t>
   </si>
   <si>
-    <t xml:space="preserve">Jihan Fahriza Amalina </t>
-  </si>
-  <si>
-    <t>099087</t>
-  </si>
-  <si>
-    <t>081111111111111</t>
+    <t>Ganti Preon</t>
+  </si>
+  <si>
+    <t>Denpoo DDS-199CI</t>
+  </si>
+  <si>
+    <t>Usep</t>
+  </si>
+  <si>
+    <t>Qarib Abdullah Shakil</t>
+  </si>
+  <si>
+    <t>08976756765</t>
+  </si>
+  <si>
+    <t>2025-06-20</t>
+  </si>
+  <si>
+    <t>Lorem Ipsum is simply dummy text of the printing and typesetting industry.</t>
+  </si>
+  <si>
+    <t>LG H05TN4</t>
   </si>
 </sst>
 </file>
@@ -442,10 +530,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -463,7 +551,7 @@
     <col min="11" max="11" width="25" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:13">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -478,7 +566,7 @@
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -493,7 +581,7 @@
       <c r="J2"/>
       <c r="K2"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:13">
       <c r="A10" s="4" t="s">
         <v>2</v>
       </c>
@@ -509,56 +597,193 @@
       <c r="E10" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="F10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:13">
       <c r="A11" s="5">
         <v>1</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="5">
-        <v>123344</v>
-      </c>
-      <c r="E11" s="5">
-        <v>123456789012</v>
+        <v>15</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11" s="5">
+        <v>27</v>
+      </c>
+      <c r="M11" s="5">
+        <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:13">
       <c r="A12" s="5">
         <v>2</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="5">
-        <v>23657</v>
-      </c>
-      <c r="E12" s="5">
-        <v>1234567890098</v>
+        <v>24</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0.09</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L12" s="5">
+        <v>26</v>
+      </c>
+      <c r="M12" s="5">
+        <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:13">
       <c r="A13" s="5">
         <v>3</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>12</v>
+        <v>31</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0.09</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>14</v>
+        <v>32</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" s="5">
+        <v>25</v>
+      </c>
+      <c r="M13" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="5">
+        <v>4</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0.12</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L14" s="5">
+        <v>24</v>
+      </c>
+      <c r="M14" s="5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>